<commit_message>
Nuevo incidente agregado - Prueba
</commit_message>
<xml_diff>
--- a/SSO_datos_ejemplo.xlsx
+++ b/SSO_datos_ejemplo.xlsx
@@ -10474,7 +10474,11 @@
           <t>Fatalidad (es) x Pasa una vez o más al año</t>
         </is>
       </c>
-      <c r="L204" t="inlineStr"/>
+      <c r="L204" t="inlineStr">
+        <is>
+          <t>12:03</t>
+        </is>
+      </c>
       <c r="M204" t="inlineStr"/>
     </row>
   </sheetData>

</xml_diff>